<commit_message>
der e planilha de arquitetura
</commit_message>
<xml_diff>
--- a/Planilha-Arquitetura.xlsx
+++ b/Planilha-Arquitetura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan.collyns.s.silva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PI\API-Acolhe-SP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4587A01-3226-4E0E-A54E-0AA592A11B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5763404D-D33F-4F2E-B6E5-7C41F38D3F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guia de Engenharia v4" sheetId="3" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
-  <si>
-    <t>O que é crítico na sua aplicação? O que gera alto impacto?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>ANÁLISE</t>
   </si>
@@ -510,6 +507,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,12 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,24 +809,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036DB22A-6FFA-4CD0-A3AA-AF0DD32AFF0D}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="121" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="56" style="1"/>
-    <col min="5" max="5" width="66.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66.85546875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="56" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="4"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2"/>
@@ -837,170 +832,170 @@
     <row r="3" spans="1:7">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="31.5">
+      <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="31">
-      <c r="A4" s="18" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.5">
+      <c r="A6" s="21"/>
+      <c r="B6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="C6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31">
-      <c r="A6" s="19"/>
-      <c r="B6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="13" t="s">
+    <row r="7" spans="1:7" ht="47.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="47.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="46.5">
-      <c r="A7" s="19"/>
-      <c r="B7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="46.5">
-      <c r="A9" s="19"/>
-      <c r="B9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="13" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="47.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="C10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="47.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.5">
+      <c r="A12" s="21"/>
+      <c r="B12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5">
+      <c r="A13" s="22"/>
+      <c r="B13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="46.5">
-      <c r="A10" s="19"/>
-      <c r="B10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="46.5">
-      <c r="A11" s="19"/>
-      <c r="B11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31">
-      <c r="A12" s="19"/>
-      <c r="B12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31">
-      <c r="A13" s="20"/>
-      <c r="B13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="E13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1010,80 +1005,80 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="69" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="62.45" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="62.5" customHeight="1">
-      <c r="A16" s="19"/>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="63">
+      <c r="A17" s="21"/>
+      <c r="B17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="47.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="55.5" customHeight="1">
+      <c r="A19" s="22"/>
+      <c r="B19" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E19" s="15" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="62">
-      <c r="A17" s="19"/>
-      <c r="B17" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="46.5">
-      <c r="A18" s="19"/>
-      <c r="B18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="55.5" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1093,110 +1088,110 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="49.5" customHeight="1">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="47.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="C22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="59.1" customHeight="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="46.5">
-      <c r="A22" s="19"/>
-      <c r="B22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="59" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="E23" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="79.5" customHeight="1">
+      <c r="A24" s="21"/>
+      <c r="B24" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="C24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="79.5" customHeight="1">
-      <c r="A24" s="19"/>
-      <c r="B24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="15" t="s">
+      <c r="E24" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="62.45" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="C25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.5" customHeight="1">
+      <c r="A26" s="21"/>
+      <c r="B26" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="62.5" customHeight="1">
-      <c r="A25" s="19"/>
-      <c r="B25" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="14" t="s">
+    <row r="27" spans="1:5" ht="47.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="46.5">
-      <c r="A27" s="20"/>
-      <c r="B27" s="13" t="s">
+      <c r="C27" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="D27" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5">

</xml_diff>